<commit_message>
Backup to GitHub - 2021.03.27
</commit_message>
<xml_diff>
--- a/02_Logistic_Regression/Output/LrBkPn_00_Results_Summary.xlsx
+++ b/02_Logistic_Regression/Output/LrBkPn_00_Results_Summary.xlsx
@@ -8,16 +8,41 @@
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="1" r:id="rId1"/>
-    <sheet name="PCA_VAR" sheetId="2" r:id="rId2"/>
-    <sheet name="PCA_Components" sheetId="3" r:id="rId3"/>
-    <sheet name="PCA_Top_Features" sheetId="4" r:id="rId4"/>
+    <sheet name="VIF" sheetId="2" r:id="rId2"/>
+    <sheet name="PCA_VAR" sheetId="3" r:id="rId3"/>
+    <sheet name="PCA_Components" sheetId="4" r:id="rId4"/>
+    <sheet name="PCA_Top_Features" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="41">
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>std</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>25%</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
+    <t>75%</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
   <si>
     <t>pelvic_incidence</t>
   </si>
@@ -58,28 +83,10 @@
     <t>Class_att</t>
   </si>
   <si>
-    <t>count</t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>std</t>
-  </si>
-  <si>
-    <t>min</t>
-  </si>
-  <si>
-    <t>25%</t>
-  </si>
-  <si>
-    <t>50%</t>
-  </si>
-  <si>
-    <t>75%</t>
-  </si>
-  <si>
-    <t>max</t>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>VIF</t>
   </si>
   <si>
     <t>PC</t>
@@ -491,13 +498,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -522,371 +529,381 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="B2">
         <v>310</v>
       </c>
       <c r="C2">
+        <v>60.497</v>
+      </c>
+      <c r="D2">
+        <v>17.237</v>
+      </c>
+      <c r="E2">
+        <v>26.148</v>
+      </c>
+      <c r="F2">
+        <v>46.43</v>
+      </c>
+      <c r="G2">
+        <v>58.692</v>
+      </c>
+      <c r="H2">
+        <v>72.878</v>
+      </c>
+      <c r="I2">
+        <v>129.834</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
         <v>310</v>
-      </c>
-      <c r="D2">
-        <v>310</v>
-      </c>
-      <c r="E2">
-        <v>310</v>
-      </c>
-      <c r="F2">
-        <v>310</v>
-      </c>
-      <c r="G2">
-        <v>310</v>
-      </c>
-      <c r="H2">
-        <v>310</v>
-      </c>
-      <c r="I2">
-        <v>310</v>
-      </c>
-      <c r="J2">
-        <v>310</v>
-      </c>
-      <c r="K2">
-        <v>310</v>
-      </c>
-      <c r="L2">
-        <v>310</v>
-      </c>
-      <c r="M2">
-        <v>310</v>
-      </c>
-      <c r="N2">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3">
-        <v>60.497</v>
       </c>
       <c r="C3">
         <v>17.543</v>
       </c>
       <c r="D3">
+        <v>10.008</v>
+      </c>
+      <c r="E3">
+        <v>-6.555</v>
+      </c>
+      <c r="F3">
+        <v>10.667</v>
+      </c>
+      <c r="G3">
+        <v>16.358</v>
+      </c>
+      <c r="H3">
+        <v>22.12</v>
+      </c>
+      <c r="I3">
+        <v>49.432</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>310</v>
+      </c>
+      <c r="C4">
         <v>51.931</v>
-      </c>
-      <c r="E3">
-        <v>42.954</v>
-      </c>
-      <c r="F3">
-        <v>117.921</v>
-      </c>
-      <c r="G3">
-        <v>26.297</v>
-      </c>
-      <c r="H3">
-        <v>0.473</v>
-      </c>
-      <c r="I3">
-        <v>21.321</v>
-      </c>
-      <c r="J3">
-        <v>13.065</v>
-      </c>
-      <c r="K3">
-        <v>11.933</v>
-      </c>
-      <c r="L3">
-        <v>-14.053</v>
-      </c>
-      <c r="M3">
-        <v>25.646</v>
-      </c>
-      <c r="N3">
-        <v>0.323</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4">
-        <v>17.237</v>
-      </c>
-      <c r="C4">
-        <v>10.008</v>
       </c>
       <c r="D4">
         <v>18.554</v>
       </c>
       <c r="E4">
+        <v>14</v>
+      </c>
+      <c r="F4">
+        <v>37</v>
+      </c>
+      <c r="G4">
+        <v>49.562</v>
+      </c>
+      <c r="H4">
+        <v>63</v>
+      </c>
+      <c r="I4">
+        <v>125.742</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>310</v>
+      </c>
+      <c r="C5">
+        <v>42.954</v>
+      </c>
+      <c r="D5">
         <v>13.423</v>
-      </c>
-      <c r="F4">
-        <v>13.317</v>
-      </c>
-      <c r="G4">
-        <v>37.559</v>
-      </c>
-      <c r="H4">
-        <v>0.286</v>
-      </c>
-      <c r="I4">
-        <v>8.638999999999999</v>
-      </c>
-      <c r="J4">
-        <v>3.4</v>
-      </c>
-      <c r="K4">
-        <v>2.893</v>
-      </c>
-      <c r="L4">
-        <v>12.226</v>
-      </c>
-      <c r="M4">
-        <v>10.451</v>
-      </c>
-      <c r="N4">
-        <v>0.468</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5">
-        <v>26.148</v>
-      </c>
-      <c r="C5">
-        <v>-6.555</v>
-      </c>
-      <c r="D5">
-        <v>14</v>
       </c>
       <c r="E5">
         <v>13.367</v>
       </c>
       <c r="F5">
+        <v>33.347</v>
+      </c>
+      <c r="G5">
+        <v>42.405</v>
+      </c>
+      <c r="H5">
+        <v>52.696</v>
+      </c>
+      <c r="I5">
+        <v>121.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>310</v>
+      </c>
+      <c r="C6">
+        <v>117.921</v>
+      </c>
+      <c r="D6">
+        <v>13.317</v>
+      </c>
+      <c r="E6">
         <v>70.083</v>
-      </c>
-      <c r="G5">
-        <v>-11.058</v>
-      </c>
-      <c r="H5">
-        <v>0.003</v>
-      </c>
-      <c r="I5">
-        <v>7.027</v>
-      </c>
-      <c r="J5">
-        <v>7.038</v>
-      </c>
-      <c r="K5">
-        <v>7.031</v>
-      </c>
-      <c r="L5">
-        <v>-35.287</v>
-      </c>
-      <c r="M5">
-        <v>7.008</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
-        <v>46.43</v>
-      </c>
-      <c r="C6">
-        <v>10.667</v>
-      </c>
-      <c r="D6">
-        <v>37</v>
-      </c>
-      <c r="E6">
-        <v>33.347</v>
       </c>
       <c r="F6">
         <v>110.709</v>
       </c>
       <c r="G6">
+        <v>118.268</v>
+      </c>
+      <c r="H6">
+        <v>125.468</v>
+      </c>
+      <c r="I6">
+        <v>163.071</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>310</v>
+      </c>
+      <c r="C7">
+        <v>26.297</v>
+      </c>
+      <c r="D7">
+        <v>37.559</v>
+      </c>
+      <c r="E7">
+        <v>-11.058</v>
+      </c>
+      <c r="F7">
         <v>1.604</v>
-      </c>
-      <c r="H6">
-        <v>0.225</v>
-      </c>
-      <c r="I6">
-        <v>13.054</v>
-      </c>
-      <c r="J6">
-        <v>10.418</v>
-      </c>
-      <c r="K6">
-        <v>9.541</v>
-      </c>
-      <c r="L6">
-        <v>-24.29</v>
-      </c>
-      <c r="M6">
-        <v>17.189</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7">
-        <v>58.692</v>
-      </c>
-      <c r="C7">
-        <v>16.358</v>
-      </c>
-      <c r="D7">
-        <v>49.562</v>
-      </c>
-      <c r="E7">
-        <v>42.405</v>
-      </c>
-      <c r="F7">
-        <v>118.268</v>
       </c>
       <c r="G7">
         <v>11.768</v>
       </c>
       <c r="H7">
+        <v>41.288</v>
+      </c>
+      <c r="I7">
+        <v>418.543</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>310</v>
+      </c>
+      <c r="C8">
+        <v>0.473</v>
+      </c>
+      <c r="D8">
+        <v>0.286</v>
+      </c>
+      <c r="E8">
+        <v>0.003</v>
+      </c>
+      <c r="F8">
+        <v>0.225</v>
+      </c>
+      <c r="G8">
         <v>0.476</v>
-      </c>
-      <c r="I7">
-        <v>21.907</v>
-      </c>
-      <c r="J7">
-        <v>12.939</v>
-      </c>
-      <c r="K7">
-        <v>11.954</v>
-      </c>
-      <c r="L7">
-        <v>-14.623</v>
-      </c>
-      <c r="M7">
-        <v>24.932</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8">
-        <v>72.878</v>
-      </c>
-      <c r="C8">
-        <v>22.12</v>
-      </c>
-      <c r="D8">
-        <v>63</v>
-      </c>
-      <c r="E8">
-        <v>52.696</v>
-      </c>
-      <c r="F8">
-        <v>125.468</v>
-      </c>
-      <c r="G8">
-        <v>41.288</v>
       </c>
       <c r="H8">
         <v>0.705</v>
       </c>
       <c r="I8">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>310</v>
+      </c>
+      <c r="C9">
+        <v>21.321</v>
+      </c>
+      <c r="D9">
+        <v>8.638999999999999</v>
+      </c>
+      <c r="E9">
+        <v>7.027</v>
+      </c>
+      <c r="F9">
+        <v>13.054</v>
+      </c>
+      <c r="G9">
+        <v>21.907</v>
+      </c>
+      <c r="H9">
         <v>28.954</v>
-      </c>
-      <c r="J8">
-        <v>15.89</v>
-      </c>
-      <c r="K8">
-        <v>14.372</v>
-      </c>
-      <c r="L8">
-        <v>-3.497</v>
-      </c>
-      <c r="M8">
-        <v>33.979</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9">
-        <v>129.834</v>
-      </c>
-      <c r="C9">
-        <v>49.432</v>
-      </c>
-      <c r="D9">
-        <v>125.742</v>
-      </c>
-      <c r="E9">
-        <v>121.43</v>
-      </c>
-      <c r="F9">
-        <v>163.071</v>
-      </c>
-      <c r="G9">
-        <v>418.543</v>
-      </c>
-      <c r="H9">
-        <v>0.999</v>
       </c>
       <c r="I9">
         <v>36.744</v>
       </c>
-      <c r="J9">
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>310</v>
+      </c>
+      <c r="C10">
+        <v>13.065</v>
+      </c>
+      <c r="D10">
+        <v>3.4</v>
+      </c>
+      <c r="E10">
+        <v>7.038</v>
+      </c>
+      <c r="F10">
+        <v>10.418</v>
+      </c>
+      <c r="G10">
+        <v>12.939</v>
+      </c>
+      <c r="H10">
+        <v>15.89</v>
+      </c>
+      <c r="I10">
         <v>19.324</v>
       </c>
-      <c r="K9">
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>310</v>
+      </c>
+      <c r="C11">
+        <v>11.933</v>
+      </c>
+      <c r="D11">
+        <v>2.893</v>
+      </c>
+      <c r="E11">
+        <v>7.031</v>
+      </c>
+      <c r="F11">
+        <v>9.541</v>
+      </c>
+      <c r="G11">
+        <v>11.954</v>
+      </c>
+      <c r="H11">
+        <v>14.372</v>
+      </c>
+      <c r="I11">
         <v>16.821</v>
       </c>
-      <c r="L9">
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>310</v>
+      </c>
+      <c r="C12">
+        <v>-14.053</v>
+      </c>
+      <c r="D12">
+        <v>12.226</v>
+      </c>
+      <c r="E12">
+        <v>-35.287</v>
+      </c>
+      <c r="F12">
+        <v>-24.29</v>
+      </c>
+      <c r="G12">
+        <v>-14.623</v>
+      </c>
+      <c r="H12">
+        <v>-3.497</v>
+      </c>
+      <c r="I12">
         <v>6.972</v>
       </c>
-      <c r="M9">
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>310</v>
+      </c>
+      <c r="C13">
+        <v>25.646</v>
+      </c>
+      <c r="D13">
+        <v>10.451</v>
+      </c>
+      <c r="E13">
+        <v>7.008</v>
+      </c>
+      <c r="F13">
+        <v>17.189</v>
+      </c>
+      <c r="G13">
+        <v>24.932</v>
+      </c>
+      <c r="H13">
+        <v>33.979</v>
+      </c>
+      <c r="I13">
         <v>44.341</v>
       </c>
-      <c r="N9">
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>310</v>
+      </c>
+      <c r="C14">
+        <v>0.323</v>
+      </c>
+      <c r="D14">
+        <v>0.468</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
         <v>1</v>
       </c>
     </row>
@@ -896,6 +913,170 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>17854564448.53867</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>1839600148.508836</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>19.55932651283906</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>9137815184.995316</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>40.25515896510515</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>2.739011001354697</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>3.819412339414828</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>7.346293972887977</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>15.24331205093313</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>17.04711841146843</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>2.338287830692853</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <v>6.960206749404332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>2.169385148926857</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -993,7 +1174,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M11"/>
   <sheetViews>
@@ -1454,7 +1635,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -1464,16 +1645,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1481,16 +1662,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>0.53</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1498,16 +1679,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>0.623</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1515,16 +1696,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D4">
         <v>0.629</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1532,16 +1713,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D5">
         <v>-0.57</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1549,16 +1730,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D6">
         <v>0.503</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1566,16 +1747,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>0.76</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1583,16 +1764,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D8">
         <v>-0.612</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1600,16 +1781,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D9">
         <v>0.534</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1617,16 +1798,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D10">
         <v>-0.598</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1634,16 +1815,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D11">
         <v>0.803</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1651,16 +1832,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D12">
         <v>0.674</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1668,16 +1849,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D13">
         <v>-0.717</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1685,16 +1866,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D14">
         <v>0.5590000000000001</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Backup to GitHub - 2021.04.03
</commit_message>
<xml_diff>
--- a/02_Logistic_Regression/Output/LrBkPn_00_Results_Summary.xlsx
+++ b/02_Logistic_Regression/Output/LrBkPn_00_Results_Summary.xlsx
@@ -1115,7 +1115,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1131,7 +1131,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.273</v>
+        <v>0.158</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1139,7 +1139,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.104</v>
+        <v>0.149</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1147,7 +1147,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.095</v>
+        <v>0.137</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1155,7 +1155,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.08799999999999999</v>
+        <v>0.126</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1163,7 +1163,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.08500000000000001</v>
+        <v>0.123</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1171,7 +1171,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.081</v>
+        <v>0.116</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1179,7 +1179,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.074</v>
+        <v>0.102</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1187,23 +1187,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.074</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>0.061</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>0.039</v>
+        <v>0.044</v>
       </c>
     </row>
   </sheetData>
@@ -1213,7 +1197,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1262,40 +1246,40 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.53</v>
+        <v>-0.056</v>
       </c>
       <c r="C2">
-        <v>0.322</v>
+        <v>-0.05</v>
       </c>
       <c r="D2">
-        <v>0.456</v>
+        <v>-0.07199999999999999</v>
       </c>
       <c r="E2">
-        <v>0.441</v>
+        <v>-0.027</v>
       </c>
       <c r="F2">
-        <v>-0.144</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>0.421</v>
+        <v>-0.039</v>
       </c>
       <c r="H2">
-        <v>0.044</v>
+        <v>-0.518</v>
       </c>
       <c r="I2">
-        <v>-0.075</v>
+        <v>-0.224</v>
       </c>
       <c r="J2">
-        <v>-0.07000000000000001</v>
+        <v>-0.105</v>
       </c>
       <c r="K2">
-        <v>0.032</v>
+        <v>-0.706</v>
       </c>
       <c r="L2">
-        <v>0.026</v>
+        <v>-0.386</v>
       </c>
       <c r="M2">
-        <v>-0.019</v>
+        <v>0.102</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1303,40 +1287,40 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-0.025</v>
+        <v>0.261</v>
       </c>
       <c r="C3">
-        <v>0.415</v>
+        <v>0.214</v>
       </c>
       <c r="D3">
-        <v>0.08599999999999999</v>
+        <v>0.248</v>
       </c>
       <c r="E3">
-        <v>-0.342</v>
+        <v>0.14</v>
       </c>
       <c r="F3">
-        <v>0.623</v>
+        <v>-0.06</v>
       </c>
       <c r="G3">
-        <v>0.157</v>
+        <v>0.1</v>
       </c>
       <c r="H3">
-        <v>0.269</v>
+        <v>0.191</v>
       </c>
       <c r="I3">
-        <v>0.1</v>
+        <v>-0.715</v>
       </c>
       <c r="J3">
-        <v>0.121</v>
+        <v>-0.263</v>
       </c>
       <c r="K3">
-        <v>0.187</v>
+        <v>-0.162</v>
       </c>
       <c r="L3">
-        <v>0.244</v>
+        <v>0.379</v>
       </c>
       <c r="M3">
-        <v>-0.315</v>
+        <v>-0.061</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1344,40 +1328,40 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-0.029</v>
+        <v>-0.079</v>
       </c>
       <c r="C4">
-        <v>-0.279</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="D4">
-        <v>-0.03</v>
+        <v>-0.057</v>
       </c>
       <c r="E4">
-        <v>0.171</v>
+        <v>-0.039</v>
       </c>
       <c r="F4">
-        <v>-0.265</v>
+        <v>-0.001</v>
       </c>
       <c r="G4">
-        <v>-0.008</v>
+        <v>-0.038</v>
       </c>
       <c r="H4">
-        <v>0.468</v>
+        <v>-0.423</v>
       </c>
       <c r="I4">
-        <v>0.308</v>
+        <v>-0.232</v>
       </c>
       <c r="J4">
-        <v>0.203</v>
+        <v>0.342</v>
       </c>
       <c r="K4">
-        <v>0.629</v>
+        <v>0.242</v>
       </c>
       <c r="L4">
-        <v>0.257</v>
+        <v>0.378</v>
       </c>
       <c r="M4">
-        <v>0.061</v>
+        <v>0.658</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1385,40 +1369,40 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.008</v>
+        <v>0.243</v>
       </c>
       <c r="C5">
-        <v>-0.073</v>
+        <v>0.174</v>
       </c>
       <c r="D5">
-        <v>-0.048</v>
+        <v>0.201</v>
       </c>
       <c r="E5">
-        <v>0.065</v>
+        <v>0.142</v>
       </c>
       <c r="F5">
-        <v>-0.076</v>
+        <v>-0.098</v>
       </c>
       <c r="G5">
-        <v>0.021</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="H5">
-        <v>0.232</v>
+        <v>-0.166</v>
       </c>
       <c r="I5">
-        <v>0.462</v>
+        <v>-0.056</v>
       </c>
       <c r="J5">
-        <v>-0.332</v>
+        <v>-0.42</v>
       </c>
       <c r="K5">
-        <v>-0.109</v>
+        <v>0.483</v>
       </c>
       <c r="L5">
-        <v>-0.518</v>
+        <v>-0.547</v>
       </c>
       <c r="M5">
-        <v>-0.57</v>
+        <v>0.306</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1426,40 +1410,40 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.066</v>
+        <v>0.028</v>
       </c>
       <c r="C6">
-        <v>0.118</v>
+        <v>0.012</v>
       </c>
       <c r="D6">
-        <v>0.041</v>
+        <v>0.003</v>
       </c>
       <c r="E6">
-        <v>-0.002</v>
+        <v>0.02</v>
       </c>
       <c r="F6">
-        <v>0.168</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>0.07099999999999999</v>
+        <v>0.001</v>
       </c>
       <c r="H6">
-        <v>-0.453</v>
+        <v>-0.132</v>
       </c>
       <c r="I6">
-        <v>0.503</v>
+        <v>0.496</v>
       </c>
       <c r="J6">
-        <v>0.429</v>
+        <v>-0.649</v>
       </c>
       <c r="K6">
-        <v>0.227</v>
+        <v>-0.193</v>
       </c>
       <c r="L6">
-        <v>-0.421</v>
+        <v>0.472</v>
       </c>
       <c r="M6">
-        <v>0.276</v>
+        <v>0.234</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1467,40 +1451,40 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-0.006</v>
+        <v>0.135</v>
       </c>
       <c r="C7">
-        <v>-0.13</v>
+        <v>0.161</v>
       </c>
       <c r="D7">
-        <v>0.027</v>
+        <v>0.153</v>
       </c>
       <c r="E7">
-        <v>0.089</v>
+        <v>0.046</v>
       </c>
       <c r="F7">
-        <v>-0.106</v>
+        <v>-0.015</v>
       </c>
       <c r="G7">
-        <v>0.006</v>
+        <v>0.048</v>
       </c>
       <c r="H7">
-        <v>0.097</v>
+        <v>-0.6820000000000001</v>
       </c>
       <c r="I7">
-        <v>-0.349</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="J7">
-        <v>0.76</v>
+        <v>0.067</v>
       </c>
       <c r="K7">
-        <v>-0.15</v>
+        <v>0.228</v>
       </c>
       <c r="L7">
-        <v>-0.194</v>
+        <v>0.205</v>
       </c>
       <c r="M7">
-        <v>-0.442</v>
+        <v>-0.599</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1508,40 +1492,40 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-0.035</v>
+        <v>-0.446</v>
       </c>
       <c r="C8">
-        <v>0.164</v>
+        <v>-0.331</v>
       </c>
       <c r="D8">
-        <v>-0.037</v>
+        <v>-0.36</v>
       </c>
       <c r="E8">
-        <v>-0.167</v>
+        <v>-0.256</v>
       </c>
       <c r="F8">
+        <v>0.055</v>
+      </c>
+      <c r="G8">
+        <v>-0.157</v>
+      </c>
+      <c r="H8">
+        <v>-0.06900000000000001</v>
+      </c>
+      <c r="I8">
+        <v>-0.359</v>
+      </c>
+      <c r="J8">
+        <v>-0.446</v>
+      </c>
+      <c r="K8">
+        <v>0.305</v>
+      </c>
+      <c r="L8">
         <v>0.018</v>
       </c>
-      <c r="G8">
-        <v>0.018</v>
-      </c>
-      <c r="H8">
-        <v>0.306</v>
-      </c>
-      <c r="I8">
-        <v>-0.48</v>
-      </c>
-      <c r="J8">
-        <v>-0.137</v>
-      </c>
-      <c r="K8">
-        <v>0.4</v>
-      </c>
-      <c r="L8">
-        <v>-0.612</v>
-      </c>
       <c r="M8">
-        <v>0.255</v>
+        <v>-0.205</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1549,122 +1533,40 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.016</v>
+        <v>0.098</v>
       </c>
       <c r="C9">
-        <v>-0.186</v>
+        <v>-0.672</v>
       </c>
       <c r="D9">
-        <v>-0.008</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="E9">
-        <v>0.16</v>
+        <v>0.442</v>
       </c>
       <c r="F9">
-        <v>0.325</v>
+        <v>-0.575</v>
       </c>
       <c r="G9">
-        <v>0.137</v>
+        <v>0.005</v>
       </c>
       <c r="H9">
-        <v>0.534</v>
+        <v>-0.016</v>
       </c>
       <c r="I9">
-        <v>0.159</v>
+        <v>0.011</v>
       </c>
       <c r="J9">
-        <v>0.141</v>
+        <v>0.02</v>
       </c>
       <c r="K9">
-        <v>-0.508</v>
+        <v>-0.006</v>
       </c>
       <c r="L9">
-        <v>-0.109</v>
+        <v>0.03</v>
       </c>
       <c r="M9">
-        <v>0.464</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>-0.125</v>
-      </c>
-      <c r="C10">
-        <v>-0.598</v>
-      </c>
-      <c r="D10">
-        <v>0.184</v>
-      </c>
-      <c r="E10">
-        <v>0.285</v>
-      </c>
-      <c r="F10">
-        <v>0.514</v>
-      </c>
-      <c r="G10">
-        <v>0.231</v>
-      </c>
-      <c r="H10">
-        <v>-0.232</v>
-      </c>
-      <c r="I10">
-        <v>-0.196</v>
-      </c>
-      <c r="J10">
-        <v>-0.172</v>
-      </c>
-      <c r="K10">
-        <v>0.234</v>
-      </c>
-      <c r="L10">
-        <v>-0.044</v>
-      </c>
-      <c r="M10">
-        <v>-0.126</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>-0.106</v>
-      </c>
-      <c r="C11">
-        <v>-0.016</v>
-      </c>
-      <c r="D11">
-        <v>-0.538</v>
-      </c>
-      <c r="E11">
-        <v>-0.125</v>
-      </c>
-      <c r="F11">
-        <v>-0.171</v>
-      </c>
-      <c r="G11">
-        <v>0.803</v>
-      </c>
-      <c r="H11">
-        <v>-0.077</v>
-      </c>
-      <c r="I11">
-        <v>-0.019</v>
-      </c>
-      <c r="J11">
-        <v>0.006</v>
-      </c>
-      <c r="K11">
-        <v>-0.02</v>
-      </c>
-      <c r="L11">
-        <v>0.047</v>
-      </c>
-      <c r="M11">
-        <v>-0.005</v>
+        <v>-0.058</v>
       </c>
     </row>
   </sheetData>

</xml_diff>